<commit_message>
exclusão de aba não utilizada
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2022/tipo_payback.xlsx
+++ b/inst/dados_premissas/2022/tipo_payback.xlsx
@@ -3,13 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676092B5-586E-48AF-A94A-82BC5F0545E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EB2B9F-AC9D-4F9E-8EFA-4F685444912C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="meses" sheetId="3" r:id="rId1"/>
-    <sheet name="fator" sheetId="2" r:id="rId2"/>
+    <sheet name="tipo" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,12 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>segmento</t>
-  </si>
-  <si>
-    <t>fator_construcao</t>
   </si>
   <si>
     <t>residencial</t>
@@ -379,128 +375,60 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="e">
-        <f>1-meses!B2/12</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="e">
-        <f>1-meses!B3/12</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="e">
-        <f>1-meses!B4/12</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="e">
-        <f>1-meses!B5/12</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="e">
-        <f>1-meses!B6/12</f>
-        <v>#VALUE!</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>